<commit_message>
Fix habit tracking for linked tasks and month navigation
- Added new /api/habits/{id}/month-data endpoint that correctly reads from DailyTimeEntry for linked tasks
- Fixed habit completion calculation to check against target values (at_least/at_most/exactly)
- Made month navigation habit-specific (each habit has independent month state)
- Fixed future dates showing as red crosses - now only past missed dates show red
- Added 'Start' text on habit start date instead of day number
- Month navigation limited: Previous disabled before habit start month, Next disabled after current month
- Fixed all habitSelectedMonth references to use per-habit state object

This fixes the Daily Speech habit tracking issue where linked task time entries weren't being recognized.
</commit_message>
<xml_diff>
--- a/docs/mytimemanager.xlsx
+++ b/docs/mytimemanager.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbiswal/projects/mytimemanager/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F69202D-9B39-8F42-9451-EC161FA862DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8ECD99B-752F-6549-8838-3E222B9DBECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="760" windowWidth="25240" windowHeight="18840" activeTab="4" xr2:uid="{1CB184EE-60AD-9B47-8E7E-3682C5F1060B}"/>
+    <workbookView xWindow="6060" yWindow="760" windowWidth="25240" windowHeight="18840" xr2:uid="{1CB184EE-60AD-9B47-8E7E-3682C5F1060B}"/>
   </bookViews>
   <sheets>
-    <sheet name="RD" sheetId="11" r:id="rId1"/>
-    <sheet name="Goal" sheetId="10" state="hidden" r:id="rId2"/>
-    <sheet name="Priority" sheetId="12" r:id="rId3"/>
-    <sheet name="Blank" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="13" r:id="rId5"/>
+    <sheet name="RD_January" sheetId="14" r:id="rId1"/>
+    <sheet name="RD" sheetId="11" r:id="rId2"/>
+    <sheet name="Goal" sheetId="10" state="hidden" r:id="rId3"/>
+    <sheet name="Priority" sheetId="12" r:id="rId4"/>
+    <sheet name="Blank" sheetId="1" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="127">
   <si>
     <t>Sl No</t>
   </si>
@@ -623,6 +624,18 @@
   </si>
   <si>
     <t>The current Must Do Task should running on the top.</t>
+  </si>
+  <si>
+    <t>The counts should be for In Progress Task. If there is a task that is Done, don't count that.</t>
+  </si>
+  <si>
+    <t>Give a search option to search all page.</t>
+  </si>
+  <si>
+    <t>Now</t>
+  </si>
+  <si>
+    <t>Remove the NOW banner or don’t fix it</t>
   </si>
 </sst>
 </file>
@@ -814,7 +827,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1184,14 +1207,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F313A6F4-B763-8744-9913-E9698B0DCD42}">
-  <dimension ref="A1:M87"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C67505D1-E601-6C4C-A2EB-D881E37E0284}">
+  <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1220,17 +1243,17 @@
     <row r="2" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="10">
-        <f>COUNTA(B4:B73)</f>
-        <v>67</v>
+        <f>COUNTA(B4:B74)</f>
+        <v>3</v>
       </c>
       <c r="C2" s="4">
-        <f>COUNTA(C4:D73)</f>
-        <v>66</v>
+        <f>COUNTA(C4:D74)</f>
+        <v>3</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4">
-        <f>COUNTA(E4:E73)</f>
-        <v>47</v>
+        <f>COUNTA(E4:E74)</f>
+        <v>0</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1285,21 +1308,13 @@
       <c r="L4" s="3"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>61</v>
-      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="6"/>
@@ -1308,21 +1323,17 @@
       <c r="L5" s="3"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="8" t="s">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>35</v>
+        <v>126</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="6"/>
@@ -1331,21 +1342,17 @@
       <c r="L6" s="3"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="38" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="8" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>36</v>
+        <v>123</v>
       </c>
       <c r="D7" s="9"/>
-      <c r="E7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="6"/>
@@ -1357,18 +1364,14 @@
     <row r="8" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="8" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>19</v>
+        <v>124</v>
       </c>
       <c r="D8" s="9"/>
-      <c r="E8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="6"/>
@@ -1377,21 +1380,13 @@
       <c r="L8" s="3"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="B9" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>58</v>
-      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="6"/>
@@ -1400,21 +1395,13 @@
       <c r="L9" s="3"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>59</v>
-      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="6"/>
@@ -1423,14 +1410,10 @@
       <c r="L10" s="3"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>84</v>
-      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -1442,14 +1425,10 @@
       <c r="L11" s="3"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>83</v>
-      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1461,21 +1440,13 @@
       <c r="L12" s="3"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
-      <c r="B13" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>63</v>
-      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="6"/>
@@ -1484,24 +1455,14 @@
       <c r="L13" s="3"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
-      <c r="B14" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>64</v>
-      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="8">
-        <v>4</v>
-      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -1509,14 +1470,10 @@
       <c r="L14" s="3"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
-      <c r="B15" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>94</v>
-      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1528,21 +1485,13 @@
       <c r="L15" s="3"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
-      <c r="B16" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>55</v>
-      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="6"/>
@@ -1551,21 +1500,13 @@
       <c r="L16" s="3"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" ht="133" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
-      <c r="B17" s="8" t="s">
-        <v>54</v>
-      </c>
+      <c r="B17" s="8"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="6"/>
@@ -1574,21 +1515,13 @@
       <c r="L17" s="3"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
-      <c r="B18" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>57</v>
-      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="6"/>
@@ -1597,14 +1530,10 @@
       <c r="L18" s="3"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
-      <c r="B19" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>121</v>
-      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1616,14 +1545,10 @@
       <c r="L19" s="3"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
-      <c r="B20" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>122</v>
-      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1635,21 +1560,13 @@
       <c r="L20" s="3"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
-      <c r="B21" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>52</v>
-      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="6"/>
@@ -1658,21 +1575,13 @@
       <c r="L21" s="3"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
-      <c r="B22" s="8" t="s">
-        <v>51</v>
-      </c>
+      <c r="B22" s="8"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="6"/>
@@ -1681,21 +1590,13 @@
       <c r="L22" s="3"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:13" ht="95" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-      <c r="B23" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>81</v>
-      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
       <c r="D23" s="9"/>
-      <c r="E23" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="6"/>
@@ -1704,14 +1605,10 @@
       <c r="L23" s="3"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
-      <c r="B24" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>82</v>
-      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
@@ -1723,14 +1620,10 @@
       <c r="L24" s="3"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
-      <c r="B25" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>85</v>
-      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
@@ -1742,14 +1635,10 @@
       <c r="L25" s="3"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
-      <c r="B26" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>88</v>
-      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
@@ -1763,9 +1652,7 @@
     </row>
     <row r="27" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
-      <c r="B27" s="8" t="s">
-        <v>51</v>
-      </c>
+      <c r="B27" s="8"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="8"/>
@@ -1778,14 +1665,10 @@
       <c r="L27" s="3"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
-      <c r="B28" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>119</v>
-      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
@@ -1797,21 +1680,13 @@
       <c r="L28" s="3"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
-      <c r="B29" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>10</v>
-      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="9"/>
       <c r="D29" s="9"/>
-      <c r="E29" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="6"/>
@@ -1820,21 +1695,13 @@
       <c r="L29" s="3"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:13" ht="76" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
-      <c r="B30" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="6"/>
@@ -1845,19 +1712,11 @@
     </row>
     <row r="31" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
-      <c r="B31" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>37</v>
-      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="6"/>
       <c r="D31" s="9"/>
-      <c r="E31" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="6"/>
@@ -1868,19 +1727,11 @@
     </row>
     <row r="32" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
-      <c r="B32" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>38</v>
-      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="6"/>
       <c r="D32" s="9"/>
-      <c r="E32" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="6"/>
@@ -1889,21 +1740,13 @@
       <c r="L32" s="3"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
-      <c r="B33" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="B33" s="8"/>
       <c r="C33" s="6"/>
-      <c r="D33" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
       <c r="I33" s="6"/>
@@ -1912,21 +1755,13 @@
       <c r="L33" s="3"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
-      <c r="B34" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="B34" s="8"/>
       <c r="C34" s="6"/>
-      <c r="D34" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="D34" s="9"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
       <c r="I34" s="6"/>
@@ -1935,21 +1770,13 @@
       <c r="L34" s="3"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="1:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
-      <c r="B35" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
       <c r="I35" s="6"/>
@@ -1958,21 +1785,13 @@
       <c r="L35" s="3"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="1:13" ht="76" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
-      <c r="B36" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="B36" s="8"/>
       <c r="C36" s="6"/>
-      <c r="D36" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
       <c r="I36" s="6"/>
@@ -1981,21 +1800,13 @@
       <c r="L36" s="3"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
-      <c r="B37" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="6"/>
       <c r="D37" s="9"/>
-      <c r="E37" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
       <c r="I37" s="6"/>
@@ -2006,19 +1817,11 @@
     </row>
     <row r="38" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
-      <c r="B38" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>41</v>
-      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="6"/>
       <c r="D38" s="9"/>
-      <c r="E38" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
       <c r="I38" s="6"/>
@@ -2027,21 +1830,13 @@
       <c r="L38" s="3"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="1:13" ht="95" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
-      <c r="B39" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="B39" s="8"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="D39" s="9"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
       <c r="I39" s="6"/>
@@ -2050,24 +1845,14 @@
       <c r="L39" s="3"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="1:13" ht="95" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
-      <c r="B40" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>71</v>
-      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="6"/>
       <c r="D40" s="9"/>
-      <c r="E40" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G40" s="8">
-        <v>3</v>
-      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
       <c r="H40" s="8"/>
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
@@ -2075,21 +1860,13 @@
       <c r="L40" s="3"/>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
-      <c r="B41" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>25</v>
-      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="9"/>
       <c r="D41" s="9"/>
-      <c r="E41" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
       <c r="I41" s="6"/>
@@ -2098,21 +1875,13 @@
       <c r="L41" s="3"/>
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
-      <c r="B42" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>26</v>
-      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="9"/>
       <c r="D42" s="9"/>
-      <c r="E42" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
       <c r="I42" s="6"/>
@@ -2121,21 +1890,13 @@
       <c r="L42" s="3"/>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
-      <c r="B43" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="9"/>
       <c r="D43" s="9"/>
-      <c r="E43" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
       <c r="I43" s="6"/>
@@ -2144,21 +1905,13 @@
       <c r="L43" s="3"/>
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="1:13" ht="95" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
-      <c r="B44" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" s="9"/>
       <c r="D44" s="9"/>
-      <c r="E44" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
       <c r="I44" s="6"/>
@@ -2167,21 +1920,13 @@
       <c r="L44" s="3"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
-      <c r="B45" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="9"/>
       <c r="D45" s="9"/>
-      <c r="E45" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="6"/>
@@ -2190,21 +1935,13 @@
       <c r="L45" s="3"/>
       <c r="M45" s="1"/>
     </row>
-    <row r="46" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
-      <c r="B46" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>46</v>
-      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="9"/>
       <c r="D46" s="9"/>
-      <c r="E46" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
       <c r="I46" s="6"/>
@@ -2213,21 +1950,13 @@
       <c r="L46" s="3"/>
       <c r="M46" s="1"/>
     </row>
-    <row r="47" spans="1:13" ht="76" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
-      <c r="B47" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>66</v>
-      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="9"/>
       <c r="D47" s="9"/>
-      <c r="E47" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
       <c r="I47" s="6"/>
@@ -2236,21 +1965,13 @@
       <c r="L47" s="3"/>
       <c r="M47" s="1"/>
     </row>
-    <row r="48" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
-      <c r="B48" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="B48" s="8"/>
+      <c r="C48" s="9"/>
       <c r="D48" s="9"/>
-      <c r="E48" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
       <c r="I48" s="6"/>
@@ -2259,21 +1980,13 @@
       <c r="L48" s="3"/>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="1:13" ht="114" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
-      <c r="B49" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>86</v>
-      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="9"/>
       <c r="D49" s="9"/>
-      <c r="E49" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
       <c r="I49" s="6"/>
@@ -2282,14 +1995,10 @@
       <c r="L49" s="3"/>
       <c r="M49" s="1"/>
     </row>
-    <row r="50" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
-      <c r="B50" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>87</v>
-      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="9"/>
       <c r="D50" s="9"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
@@ -2301,14 +2010,10 @@
       <c r="L50" s="3"/>
       <c r="M50" s="1"/>
     </row>
-    <row r="51" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
-      <c r="B51" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>89</v>
-      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="9"/>
       <c r="D51" s="9"/>
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
@@ -2320,14 +2025,10 @@
       <c r="L51" s="3"/>
       <c r="M51" s="1"/>
     </row>
-    <row r="52" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
-      <c r="B52" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>95</v>
-      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="9"/>
       <c r="D52" s="9"/>
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
@@ -2339,14 +2040,10 @@
       <c r="L52" s="3"/>
       <c r="M52" s="1"/>
     </row>
-    <row r="53" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
-      <c r="B53" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>96</v>
-      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="9"/>
       <c r="D53" s="9"/>
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
@@ -2358,14 +2055,10 @@
       <c r="L53" s="3"/>
       <c r="M53" s="1"/>
     </row>
-    <row r="54" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
-      <c r="B54" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>120</v>
-      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="9"/>
       <c r="D54" s="9"/>
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
@@ -2377,21 +2070,13 @@
       <c r="L54" s="3"/>
       <c r="M54" s="1"/>
     </row>
-    <row r="55" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
-      <c r="B55" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="B55" s="8"/>
+      <c r="C55" s="9"/>
       <c r="D55" s="9"/>
-      <c r="E55" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
       <c r="I55" s="6"/>
@@ -2400,21 +2085,13 @@
       <c r="L55" s="3"/>
       <c r="M55" s="1"/>
     </row>
-    <row r="56" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
-      <c r="B56" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="B56" s="8"/>
       <c r="C56" s="9"/>
-      <c r="D56" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E56" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F56" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="D56" s="9"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
       <c r="I56" s="6"/>
@@ -2423,21 +2100,13 @@
       <c r="L56" s="3"/>
       <c r="M56" s="1"/>
     </row>
-    <row r="57" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
-      <c r="B57" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>47</v>
-      </c>
+      <c r="B57" s="8"/>
+      <c r="C57" s="9"/>
       <c r="D57" s="9"/>
-      <c r="E57" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F57" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
       <c r="G57" s="8"/>
       <c r="H57" s="8"/>
       <c r="I57" s="6"/>
@@ -2446,21 +2115,13 @@
       <c r="L57" s="3"/>
       <c r="M57" s="1"/>
     </row>
-    <row r="58" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
-      <c r="B58" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="B58" s="8"/>
       <c r="C58" s="9"/>
-      <c r="D58" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E58" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F58" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="D58" s="9"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
       <c r="I58" s="6"/>
@@ -2469,21 +2130,13 @@
       <c r="L58" s="3"/>
       <c r="M58" s="1"/>
     </row>
-    <row r="59" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
-      <c r="B59" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>49</v>
-      </c>
+      <c r="B59" s="8"/>
+      <c r="C59" s="9"/>
       <c r="D59" s="9"/>
-      <c r="E59" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F59" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
       <c r="I59" s="6"/>
@@ -2492,21 +2145,13 @@
       <c r="L59" s="3"/>
       <c r="M59" s="1"/>
     </row>
-    <row r="60" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
-      <c r="B60" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="B60" s="8"/>
       <c r="C60" s="9"/>
-      <c r="D60" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F60" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="D60" s="9"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
       <c r="G60" s="8"/>
       <c r="H60" s="8"/>
       <c r="I60" s="6"/>
@@ -2515,21 +2160,13 @@
       <c r="L60" s="3"/>
       <c r="M60" s="1"/>
     </row>
-    <row r="61" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
-      <c r="B61" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>68</v>
-      </c>
+      <c r="B61" s="8"/>
+      <c r="C61" s="9"/>
       <c r="D61" s="9"/>
-      <c r="E61" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F61" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
       <c r="G61" s="8"/>
       <c r="H61" s="8"/>
       <c r="I61" s="6"/>
@@ -2538,21 +2175,13 @@
       <c r="L61" s="3"/>
       <c r="M61" s="1"/>
     </row>
-    <row r="62" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
-      <c r="B62" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="B62" s="8"/>
+      <c r="C62" s="9"/>
       <c r="D62" s="9"/>
-      <c r="E62" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F62" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
       <c r="I62" s="6"/>
@@ -2561,21 +2190,13 @@
       <c r="L62" s="3"/>
       <c r="M62" s="1"/>
     </row>
-    <row r="63" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
-      <c r="B63" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="B63" s="8"/>
       <c r="C63" s="9"/>
-      <c r="D63" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E63" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F63" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="D63" s="9"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
       <c r="G63" s="8"/>
       <c r="H63" s="8"/>
       <c r="I63" s="6"/>
@@ -2584,24 +2205,14 @@
       <c r="L63" s="3"/>
       <c r="M63" s="1"/>
     </row>
-    <row r="64" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
-      <c r="B64" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>69</v>
-      </c>
+      <c r="B64" s="8"/>
+      <c r="C64" s="9"/>
       <c r="D64" s="9"/>
-      <c r="E64" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F64" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G64" s="8">
-        <v>4</v>
-      </c>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
       <c r="H64" s="8"/>
       <c r="I64" s="6"/>
       <c r="J64" s="6"/>
@@ -2609,24 +2220,14 @@
       <c r="L64" s="3"/>
       <c r="M64" s="1"/>
     </row>
-    <row r="65" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
-      <c r="B65" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>75</v>
-      </c>
+      <c r="B65" s="8"/>
+      <c r="C65" s="9"/>
       <c r="D65" s="9"/>
-      <c r="E65" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F65" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G65" s="8">
-        <v>3</v>
-      </c>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
       <c r="H65" s="8"/>
       <c r="I65" s="6"/>
       <c r="J65" s="6"/>
@@ -2634,24 +2235,14 @@
       <c r="L65" s="3"/>
       <c r="M65" s="1"/>
     </row>
-    <row r="66" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
-      <c r="B66" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>74</v>
-      </c>
+      <c r="B66" s="8"/>
+      <c r="C66" s="9"/>
       <c r="D66" s="9"/>
-      <c r="E66" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F66" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G66" s="8">
-        <v>4</v>
-      </c>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
       <c r="H66" s="8"/>
       <c r="I66" s="6"/>
       <c r="J66" s="6"/>
@@ -2659,14 +2250,10 @@
       <c r="L66" s="3"/>
       <c r="M66" s="1"/>
     </row>
-    <row r="67" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
-      <c r="B67" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>118</v>
-      </c>
+      <c r="B67" s="8"/>
+      <c r="C67" s="9"/>
       <c r="D67" s="9"/>
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
@@ -2678,14 +2265,10 @@
       <c r="L67" s="3"/>
       <c r="M67" s="1"/>
     </row>
-    <row r="68" spans="1:13" ht="76" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
-      <c r="B68" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>90</v>
-      </c>
+      <c r="B68" s="8"/>
+      <c r="C68" s="9"/>
       <c r="D68" s="9"/>
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
@@ -2697,14 +2280,10 @@
       <c r="L68" s="3"/>
       <c r="M68" s="1"/>
     </row>
-    <row r="69" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
-      <c r="B69" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>91</v>
-      </c>
+      <c r="B69" s="8"/>
+      <c r="C69" s="9"/>
       <c r="D69" s="9"/>
       <c r="E69" s="8"/>
       <c r="F69" s="8"/>
@@ -2716,14 +2295,10 @@
       <c r="L69" s="3"/>
       <c r="M69" s="1"/>
     </row>
-    <row r="70" spans="1:13" ht="76" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
-      <c r="B70" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>92</v>
-      </c>
+      <c r="B70" s="8"/>
+      <c r="C70" s="9"/>
       <c r="D70" s="9"/>
       <c r="E70" s="8"/>
       <c r="F70" s="8"/>
@@ -2735,19 +2310,1957 @@
       <c r="L70" s="3"/>
       <c r="M70" s="1"/>
     </row>
-    <row r="71" spans="1:13" ht="76" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
-      <c r="B71" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>93</v>
-      </c>
+      <c r="B71" s="8"/>
+      <c r="C71" s="9"/>
       <c r="D71" s="9"/>
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
       <c r="G71" s="8"/>
       <c r="H71" s="8"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="6"/>
+      <c r="K71" s="6"/>
+      <c r="L71" s="3"/>
+      <c r="M71" s="1"/>
+    </row>
+    <row r="72" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A72" s="2"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="6"/>
+      <c r="J72" s="6"/>
+      <c r="K72" s="6"/>
+      <c r="L72" s="3"/>
+      <c r="M72" s="1"/>
+    </row>
+    <row r="73" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="2"/>
+      <c r="B73" s="8"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="6"/>
+      <c r="K73" s="6"/>
+      <c r="L73" s="3"/>
+      <c r="M73" s="1"/>
+    </row>
+    <row r="74" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="2"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="8"/>
+      <c r="F74" s="8"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="3"/>
+      <c r="M74" s="1"/>
+    </row>
+    <row r="75" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="1"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+    </row>
+    <row r="76" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+    </row>
+    <row r="77" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="1"/>
+    </row>
+    <row r="78" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="M78" s="1"/>
+    </row>
+    <row r="79" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+      <c r="K79" s="1"/>
+      <c r="L79" s="1"/>
+      <c r="M79" s="1"/>
+    </row>
+    <row r="80" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="K80" s="1"/>
+      <c r="L80" s="1"/>
+      <c r="M80" s="1"/>
+    </row>
+    <row r="81" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
+      <c r="L81" s="1"/>
+      <c r="M81" s="1"/>
+    </row>
+    <row r="82" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="1"/>
+      <c r="M82" s="1"/>
+    </row>
+    <row r="83" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+      <c r="L83" s="1"/>
+      <c r="M83" s="1"/>
+    </row>
+    <row r="84" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+      <c r="L84" s="1"/>
+      <c r="M84" s="1"/>
+    </row>
+    <row r="85" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+      <c r="K85" s="1"/>
+      <c r="L85" s="1"/>
+      <c r="M85" s="1"/>
+    </row>
+    <row r="86" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
+      <c r="L86" s="1"/>
+      <c r="M86" s="1"/>
+    </row>
+    <row r="87" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <conditionalFormatting sqref="B4:K74">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>$H4="Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F313A6F4-B763-8744-9913-E9698B0DCD42}">
+  <dimension ref="A1:M87"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D68" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.83203125" customWidth="1"/>
+    <col min="4" max="4" width="81.33203125" customWidth="1"/>
+    <col min="15" max="15" width="31.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="10">
+        <f>COUNTA(B4:B73)</f>
+        <v>67</v>
+      </c>
+      <c r="C2" s="4">
+        <f>COUNTA(C4:D73)</f>
+        <v>66</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4">
+        <f>COUNTA(E4:E73)</f>
+        <v>47</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="8">
+        <v>4</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" ht="133" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" ht="95" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="1"/>
+    </row>
+    <row r="29" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="1:13" ht="76" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="E31" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="9"/>
+      <c r="E32" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="1"/>
+    </row>
+    <row r="33" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="1"/>
+    </row>
+    <row r="34" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="1"/>
+    </row>
+    <row r="35" spans="1:13" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="B35" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="1"/>
+    </row>
+    <row r="36" spans="1:13" ht="76" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
+      <c r="B36" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="1"/>
+    </row>
+    <row r="37" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2"/>
+      <c r="B37" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="9"/>
+      <c r="E37" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="1"/>
+    </row>
+    <row r="38" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+      <c r="B38" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="9"/>
+      <c r="E38" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="1"/>
+    </row>
+    <row r="39" spans="1:13" ht="95" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+      <c r="B39" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="6"/>
+      <c r="D39" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="1"/>
+    </row>
+    <row r="40" spans="1:13" ht="95" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+      <c r="B40" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G40" s="8">
+        <v>3</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="1"/>
+    </row>
+    <row r="41" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+      <c r="A41" s="2"/>
+      <c r="B41" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="9"/>
+      <c r="E41" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="1"/>
+    </row>
+    <row r="42" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A42" s="2"/>
+      <c r="B42" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="9"/>
+      <c r="E42" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="1"/>
+    </row>
+    <row r="43" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A43" s="2"/>
+      <c r="B43" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" s="9"/>
+      <c r="E43" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="1"/>
+    </row>
+    <row r="44" spans="1:13" ht="95" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" s="9"/>
+      <c r="E44" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="1"/>
+    </row>
+    <row r="45" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A45" s="2"/>
+      <c r="B45" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" s="9"/>
+      <c r="E45" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="1"/>
+    </row>
+    <row r="46" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+      <c r="A46" s="2"/>
+      <c r="B46" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" s="9"/>
+      <c r="E46" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="1"/>
+    </row>
+    <row r="47" spans="1:13" ht="76" x14ac:dyDescent="0.2">
+      <c r="A47" s="2"/>
+      <c r="B47" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="1"/>
+    </row>
+    <row r="48" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+      <c r="A48" s="2"/>
+      <c r="B48" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48" s="9"/>
+      <c r="E48" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="1"/>
+    </row>
+    <row r="49" spans="1:13" ht="114" x14ac:dyDescent="0.2">
+      <c r="A49" s="2"/>
+      <c r="B49" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="9"/>
+      <c r="E49" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="6"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="1"/>
+    </row>
+    <row r="50" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A50" s="2"/>
+      <c r="B50" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" s="9"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I50" s="6"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="6"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="1"/>
+    </row>
+    <row r="51" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A51" s="2"/>
+      <c r="B51" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51" s="9"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="1"/>
+    </row>
+    <row r="52" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A52" s="2"/>
+      <c r="B52" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" s="9"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="1"/>
+    </row>
+    <row r="53" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A53" s="2"/>
+      <c r="B53" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D53" s="9"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="1"/>
+    </row>
+    <row r="54" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A54" s="2"/>
+      <c r="B54" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D54" s="9"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="1"/>
+    </row>
+    <row r="55" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A55" s="2"/>
+      <c r="B55" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D55" s="9"/>
+      <c r="E55" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="6"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="1"/>
+    </row>
+    <row r="56" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A56" s="2"/>
+      <c r="B56" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I56" s="6"/>
+      <c r="J56" s="6"/>
+      <c r="K56" s="6"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="1"/>
+    </row>
+    <row r="57" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+      <c r="A57" s="2"/>
+      <c r="B57" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" s="9"/>
+      <c r="E57" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I57" s="6"/>
+      <c r="J57" s="6"/>
+      <c r="K57" s="6"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="1"/>
+    </row>
+    <row r="58" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A58" s="2"/>
+      <c r="B58" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I58" s="6"/>
+      <c r="J58" s="6"/>
+      <c r="K58" s="6"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="1"/>
+    </row>
+    <row r="59" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A59" s="2"/>
+      <c r="B59" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D59" s="9"/>
+      <c r="E59" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="6"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="1"/>
+    </row>
+    <row r="60" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A60" s="2"/>
+      <c r="B60" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I60" s="6"/>
+      <c r="J60" s="6"/>
+      <c r="K60" s="6"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="1"/>
+    </row>
+    <row r="61" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+      <c r="A61" s="2"/>
+      <c r="B61" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D61" s="9"/>
+      <c r="E61" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I61" s="6"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="6"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="1"/>
+    </row>
+    <row r="62" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A62" s="2"/>
+      <c r="B62" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" s="9"/>
+      <c r="E62" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="6"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="1"/>
+    </row>
+    <row r="63" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2"/>
+      <c r="B63" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="L63" s="3"/>
+      <c r="M63" s="1"/>
+    </row>
+    <row r="64" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+      <c r="A64" s="2"/>
+      <c r="B64" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D64" s="9"/>
+      <c r="E64" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G64" s="8">
+        <v>4</v>
+      </c>
+      <c r="H64" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="L64" s="3"/>
+      <c r="M64" s="1"/>
+    </row>
+    <row r="65" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A65" s="2"/>
+      <c r="B65" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D65" s="9"/>
+      <c r="E65" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G65" s="8">
+        <v>3</v>
+      </c>
+      <c r="H65" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="3"/>
+      <c r="M65" s="1"/>
+    </row>
+    <row r="66" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A66" s="2"/>
+      <c r="B66" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D66" s="9"/>
+      <c r="E66" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G66" s="8">
+        <v>4</v>
+      </c>
+      <c r="H66" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I66" s="6"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="1"/>
+    </row>
+    <row r="67" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A67" s="2"/>
+      <c r="B67" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D67" s="9"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="1"/>
+    </row>
+    <row r="68" spans="1:13" ht="76" x14ac:dyDescent="0.2">
+      <c r="A68" s="2"/>
+      <c r="B68" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D68" s="9"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I68" s="6"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="1"/>
+    </row>
+    <row r="69" spans="1:13" ht="38" x14ac:dyDescent="0.2">
+      <c r="A69" s="2"/>
+      <c r="B69" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D69" s="9"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I69" s="6"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
+      <c r="L69" s="3"/>
+      <c r="M69" s="1"/>
+    </row>
+    <row r="70" spans="1:13" ht="76" x14ac:dyDescent="0.2">
+      <c r="A70" s="2"/>
+      <c r="B70" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D70" s="9"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I70" s="6"/>
+      <c r="J70" s="6"/>
+      <c r="K70" s="6"/>
+      <c r="L70" s="3"/>
+      <c r="M70" s="1"/>
+    </row>
+    <row r="71" spans="1:13" ht="76" x14ac:dyDescent="0.2">
+      <c r="A71" s="2"/>
+      <c r="B71" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D71" s="9"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="I71" s="6"/>
       <c r="J71" s="6"/>
       <c r="K71" s="6"/>
@@ -2977,7 +4490,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E79D08A1-EDEE-B44A-832A-B4E3F94AC1A0}">
   <dimension ref="A1:L26"/>
   <sheetViews>
@@ -3355,7 +4868,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E40C837-0071-4949-A1E8-BC974A2D0519}">
   <dimension ref="A1:M70"/>
   <sheetViews>
@@ -4335,7 +5848,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5AEF622-906B-6549-8729-A44951A33388}">
   <dimension ref="A1:R37"/>
   <sheetViews>
@@ -4957,11 +6470,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69893CEA-862A-0946-8520-D9E2EF7551E8}">
   <dimension ref="F16:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>

</xml_diff>